<commit_message>
Add input files for all courses
</commit_message>
<xml_diff>
--- a/test/13.xlsx
+++ b/test/13.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\server32-sch\Benutzerdaten$\2014\sigmunczykn\Desktop\CourseSelection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11535" tabRatio="1000" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" tabRatio="1000" firstSheet="18" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="13ade" sheetId="1" r:id="rId1"/>
@@ -41,19 +41,13 @@
     <sheet name="13Sem2" sheetId="27" r:id="rId27"/>
     <sheet name="13Sem3" sheetId="28" r:id="rId28"/>
     <sheet name="13spaF" sheetId="29" r:id="rId29"/>
-    <sheet name="13spo11" sheetId="30" r:id="rId30"/>
-    <sheet name="13spo12" sheetId="31" r:id="rId31"/>
-    <sheet name="13spo13" sheetId="32" r:id="rId32"/>
-    <sheet name="13spo21" sheetId="33" r:id="rId33"/>
-    <sheet name="13spo22" sheetId="34" r:id="rId34"/>
-    <sheet name="13spo23" sheetId="35" r:id="rId35"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="73">
   <si>
     <t>Nr.</t>
   </si>
@@ -272,47 +266,14 @@
   </si>
   <si>
     <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
@@ -491,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -522,12 +483,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -808,9 +763,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -946,6 +903,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -955,9 +917,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1110,11 +1074,16 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>69</v>
+      <c r="A19">
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1126,9 +1095,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1304,6 +1275,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1313,9 +1289,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1475,6 +1453,11 @@
         <v>59</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1484,9 +1467,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1614,6 +1599,11 @@
         <v>29</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1623,9 +1613,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1737,6 +1729,11 @@
         <v>68</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1746,9 +1743,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1924,6 +1923,11 @@
         <v>59</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1933,9 +1937,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2095,6 +2101,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2104,9 +2115,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2266,6 +2279,11 @@
         <v>63</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2275,9 +2293,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2405,6 +2425,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2414,9 +2439,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2552,6 +2579,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2561,9 +2593,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2699,6 +2733,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2708,9 +2747,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2814,6 +2855,11 @@
         <v>59</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2823,9 +2869,11 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3009,6 +3057,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3018,9 +3071,11 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3116,6 +3171,11 @@
         <v>50</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3125,9 +3185,11 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3263,6 +3325,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3272,9 +3339,11 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3370,6 +3439,11 @@
         <v>25</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3379,9 +3453,11 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3509,6 +3585,11 @@
         <v>59</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3518,9 +3599,11 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3656,6 +3739,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3665,9 +3753,11 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3827,6 +3917,11 @@
         <v>59</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3836,9 +3931,11 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3990,6 +4087,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3999,9 +4101,11 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4089,6 +4193,11 @@
         <v>59</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4098,9 +4207,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4236,566 +4347,9 @@
         <v>31</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>1</v>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4807,9 +4361,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4961,6 +4517,11 @@
         <v>50</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4970,9 +4531,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5124,6 +4687,11 @@
         <v>50</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5133,9 +4701,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5279,6 +4849,11 @@
         <v>59</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5288,9 +4863,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5410,6 +4987,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5419,9 +5001,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5573,6 +5157,11 @@
         <v>50</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5582,9 +5171,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5744,6 +5335,11 @@
         <v>59</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.39369999999999999" right="0.39369999999999999" top="0.39369999999999999" bottom="0.39369999999999999" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>